<commit_message>
Code structuring and debugging. Added type annotations and docstrings
</commit_message>
<xml_diff>
--- a/models_comparison.xlsx
+++ b/models_comparison.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaia/Desktop/gaia/individual_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24065855-BF42-6646-BDDA-B6978AA7C7F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7C69BF-DD73-0E4C-9CC2-3D108F16AF2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47720" yWindow="-24800" windowWidth="27240" windowHeight="16260" xr2:uid="{A52B3F5B-354A-114D-84DF-B9DEF105F877}"/>
+    <workbookView xWindow="22080" yWindow="-22720" windowWidth="29220" windowHeight="16040" xr2:uid="{A52B3F5B-354A-114D-84DF-B9DEF105F877}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -73,7 +73,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -113,7 +113,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,7 +451,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -489,7 +489,8 @@
         <v>0.78649999999999998</v>
       </c>
       <c r="E2" s="2">
-        <v>0.78280000000000005</v>
+        <f>2*(C2*D2)/(C2+D2)</f>
+        <v>0.7890417590773714</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -500,14 +501,15 @@
       <c r="B3" s="2">
         <v>0.76512455940246504</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>0.77869999999999995</v>
       </c>
       <c r="D3" s="2">
         <v>0.7651</v>
       </c>
-      <c r="E3" s="1">
-        <v>0.76239999999999997</v>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E7" si="0">2*(C3*D3)/(C3+D3)</f>
+        <v>0.77184009586734015</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -515,17 +517,18 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
-        <v>0.80427044630050604</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.80320000000000003</v>
+      <c r="B4" s="2">
+        <v>0.81494659185409501</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.84060000000000001</v>
       </c>
       <c r="D4" s="2">
-        <v>0.80430000000000001</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.80330000000000001</v>
+        <v>0.81489999999999996</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.82755051646028388</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -533,17 +536,18 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
-        <v>0.81494659185409501</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.81469999999999998</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.81489999999999996</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.81320000000000003</v>
+      <c r="B5" s="2">
+        <v>0.78291815519332797</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.78939999999999999</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.78290000000000004</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.78613656426890544</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -551,17 +555,18 @@
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1">
-        <v>0.77580070495605402</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.80149999999999999</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.77580000000000005</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.76980000000000004</v>
+      <c r="B6" s="2">
+        <v>0.79003560543060303</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.78849999999999998</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.78924928729806776</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -570,16 +575,17 @@
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>0.72241991758346502</v>
+        <v>0.72953736782073897</v>
       </c>
       <c r="C7" s="2">
-        <v>0.73119999999999996</v>
+        <v>0.73870000000000002</v>
       </c>
       <c r="D7" s="2">
-        <v>0.72240000000000004</v>
+        <v>0.72950000000000004</v>
       </c>
       <c r="E7" s="2">
-        <v>0.71650000000000003</v>
+        <f t="shared" si="0"/>
+        <v>0.7340711755891568</v>
       </c>
       <c r="F7" s="1"/>
     </row>

</xml_diff>